<commit_message>
finalized models for ptl, input model results i ntables that I'll bring into MS draft, and made preliminary figures for PTL, which I will have to go back and remake in ggplot so they are prettier. I also went back into the raw data and found an error: a low-risk treatment (Trial 3, reef 11) had a FHASE listed as being in a sublethal position, which is not possible. I changed it in excel
</commit_message>
<xml_diff>
--- a/2018.data.for.analyses.R/2018.predator.time.lapse/Data/2019.1.2.ptl.raw.data.xlsx
+++ b/2018.data.for.analyses.R/2018.predator.time.lapse/Data/2019.1.2.ptl.raw.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Desktop\2018 summer\2018 Goby\Goby_reproduction_by_risk\2018.data.for.analyses.R\2018.predator.time.lapse\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ECD02D-386E-474D-BFFB-D76DBA12EE4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A59286-EDCA-459A-BC05-8ACC20DF6C8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C0BCFE-E134-49E3-B781-93A364DB5B2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{27C0BCFE-E134-49E3-B781-93A364DB5B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="29">
   <si>
     <t>Trial</t>
   </si>
@@ -67207,7 +67207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3221BF15-2B44-491F-8075-B08B27C63447}">
   <dimension ref="A3:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -68211,9 +68211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6789F088-9E7F-4A1E-B30E-BD32BDD4BBA4}">
   <dimension ref="A1:H2427"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E122" sqref="E122:E131"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A360" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G379" sqref="G379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78043,7 +78043,7 @@
         <v>1</v>
       </c>
       <c r="G378" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H378" s="1">
         <v>0</v>

</xml_diff>